<commit_message>
Modification to real experiments
</commit_message>
<xml_diff>
--- a/source/experiments/complete_analysis.xlsx
+++ b/source/experiments/complete_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\TDG Matemáticas\secure-svm\source\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D0402D-4CBF-465F-B0CD-F5E0151B9CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F1B00E-6364-4B2D-845A-E9BCF4691D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B0E6BF9-C349-44B2-B939-B204AB282E45}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{7B0E6BF9-C349-44B2-B939-B204AB282E45}"/>
   </bookViews>
   <sheets>
     <sheet name="Rows experiment" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Rows</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>Num products</t>
+  </si>
+  <si>
+    <t>Times slower</t>
+  </si>
+  <si>
+    <t>Number of products</t>
+  </si>
+  <si>
+    <t>Mean Sec</t>
+  </si>
+  <si>
+    <t>Std Sec</t>
   </si>
 </sst>
 </file>
@@ -434,6 +446,7 @@
         <c:axId val="1540038959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -731,6 +744,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Secure vs. Clear)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -968,6 +1011,7 @@
         <c:axId val="1032222176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.70000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -985,6 +1029,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Training accuracy (secure)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1030,6 +1129,7 @@
         <c:axId val="1031592096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.70000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1047,6 +1147,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Training accuracy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> (clear)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4932,6 +5092,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of products vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>. Data sent</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5014,44 +5204,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.7274496937882764E-2"/>
-                  <c:y val="-6.2856882473024206E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -5273,6 +5427,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Data sent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5335,6 +5549,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> of products</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5716,6 +5990,7 @@
         <c:axId val="785002128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.75000000000000011"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5733,6 +6008,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> accuracy (secure)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5778,6 +6113,7 @@
         <c:axId val="599032240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.75000000000000011"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5795,6 +6131,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> accuracy (clear)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -15665,7 +16061,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Num products</c:v>
+                  <c:v>Number of products</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16338,7 +16734,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Num products</c:v>
+                  <c:v>Number of products</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16794,7 +17190,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Num products</c:v>
+                  <c:v>Number of products</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17174,6 +17570,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Data sent v</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>s. Number of products</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17218,7 +17644,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Num products</c:v>
+                  <c:v>Number of products</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17256,38 +17682,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -17472,6 +17868,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Data sent</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -17534,6 +17990,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Number of products</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -17686,7 +18197,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Num products</c:v>
+                  <c:v>Number of products</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17724,38 +18235,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -18110,6 +18591,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Data sent vs.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0"/>
+              <a:t> Training time</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18192,38 +18703,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -18408,6 +18889,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -18470,6 +19011,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Data</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> sent (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -33023,16 +33624,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>93760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>98397</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>390940</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>128877</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33059,16 +33660,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95748</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>112644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>707999</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>112644</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33095,16 +33696,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>139148</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>125895</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>853440</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>595023</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>993</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33131,16 +33732,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>299830</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>166646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>166315</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>72555</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33275,16 +33876,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>99392</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>53010</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>172276</xdr:rowOff>
+      <xdr:rowOff>132520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>695740</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>649358</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>132520</xdr:rowOff>
+      <xdr:rowOff>92764</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33942,13 +34543,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>3463</xdr:colOff>
+      <xdr:colOff>3464</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>62345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>131620</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>145473</xdr:rowOff>
     </xdr:to>
@@ -34275,10 +34876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429AE350-CED3-47D3-BE49-B53720A048B9}">
-  <dimension ref="B2:N23"/>
+  <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O66" sqref="O66"/>
+    <sheetView topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34295,9 +34896,10 @@
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -34335,10 +34937,13 @@
         <v>11</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>40</v>
       </c>
@@ -34379,8 +34984,12 @@
         <f>B3*B3*(C3+2)+B3+50*(4*(B3+1)*(B3+1) + 2*(B3+1)+1)</f>
         <v>346790</v>
       </c>
+      <c r="O3">
+        <f>J3/K3</f>
+        <v>72.254144693377711</v>
+      </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>40</v>
       </c>
@@ -34418,11 +35027,15 @@
         <v>3543.98</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N22" si="0">B4*B4*(C4+2)+B4+50*(4*(B4+1)*(B4+1) + 2*(B4+1)+1)</f>
+        <f>B4*B4*(C4+2)+B4+50*(4*(B4+1)*(B4+1) + 2*(B4+1)+1)</f>
         <v>346790</v>
       </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O23" si="0">J4/K4</f>
+        <v>77.761142445969796</v>
+      </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>40</v>
       </c>
@@ -34460,11 +35073,15 @@
         <v>3543.98</v>
       </c>
       <c r="N5">
+        <f t="shared" ref="N5:N22" si="1">B5*B5*(C5+2)+B5+50*(4*(B5+1)*(B5+1) + 2*(B5+1)+1)</f>
+        <v>346790</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="0"/>
-        <v>346790</v>
+        <v>83.347968329672142</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>50</v>
       </c>
@@ -34502,11 +35119,15 @@
         <v>5886.2</v>
       </c>
       <c r="N6">
+        <f t="shared" si="1"/>
+        <v>535400</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="0"/>
-        <v>535400</v>
+        <v>73.992331655883063</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>50</v>
       </c>
@@ -34544,11 +35165,15 @@
         <v>5886.2</v>
       </c>
       <c r="N7">
+        <f t="shared" si="1"/>
+        <v>535400</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="0"/>
-        <v>535400</v>
+        <v>80.460099863822066</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>50</v>
       </c>
@@ -34586,11 +35211,15 @@
         <v>5886.2</v>
       </c>
       <c r="N8">
+        <f t="shared" si="1"/>
+        <v>535400</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="0"/>
-        <v>535400</v>
+        <v>91.376108160739108</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>60</v>
       </c>
@@ -34628,11 +35257,15 @@
         <v>9047.2099999999991</v>
       </c>
       <c r="N9">
+        <f t="shared" si="1"/>
+        <v>764810</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="0"/>
-        <v>764810</v>
+        <v>93.339516533120076</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>60</v>
       </c>
@@ -34670,11 +35303,15 @@
         <v>9047.2099999999991</v>
       </c>
       <c r="N10">
+        <f t="shared" si="1"/>
+        <v>764810</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="0"/>
-        <v>764810</v>
+        <v>90.180419827922805</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>60</v>
       </c>
@@ -34712,11 +35349,15 @@
         <v>9047.2099999999991</v>
       </c>
       <c r="N11">
+        <f t="shared" si="1"/>
+        <v>764810</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="0"/>
-        <v>764810</v>
+        <v>90.548557189079361</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>70</v>
       </c>
@@ -34754,11 +35395,15 @@
         <v>12356.9</v>
       </c>
       <c r="N12">
+        <f t="shared" si="1"/>
+        <v>1035020</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="0"/>
-        <v>1035020</v>
+        <v>91.393537485520397</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>70</v>
       </c>
@@ -34796,11 +35441,15 @@
         <v>12356.9</v>
       </c>
       <c r="N13">
+        <f t="shared" si="1"/>
+        <v>1035020</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="0"/>
-        <v>1035020</v>
+        <v>97.816822450503153</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>70</v>
       </c>
@@ -34838,11 +35487,15 @@
         <v>12356.9</v>
       </c>
       <c r="N14">
+        <f t="shared" si="1"/>
+        <v>1035020</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="0"/>
-        <v>1035020</v>
+        <v>95.607889642737533</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>80</v>
       </c>
@@ -34880,11 +35533,15 @@
         <v>17284.400000000001</v>
       </c>
       <c r="N15">
+        <f t="shared" si="1"/>
+        <v>1346030</v>
+      </c>
+      <c r="O15">
         <f t="shared" si="0"/>
-        <v>1346030</v>
+        <v>90.713237497406894</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>80</v>
       </c>
@@ -34922,11 +35579,15 @@
         <v>17284.400000000001</v>
       </c>
       <c r="N16">
+        <f t="shared" si="1"/>
+        <v>1346030</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="0"/>
-        <v>1346030</v>
+        <v>92.968395141320755</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>80</v>
       </c>
@@ -34964,11 +35625,15 @@
         <v>17284.400000000001</v>
       </c>
       <c r="N17">
+        <f t="shared" si="1"/>
+        <v>1346030</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="0"/>
-        <v>1346030</v>
+        <v>97.095792783157592</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>90</v>
       </c>
@@ -35006,11 +35671,15 @@
         <v>22036.7</v>
       </c>
       <c r="N18">
+        <f t="shared" si="1"/>
+        <v>1697840</v>
+      </c>
+      <c r="O18">
         <f t="shared" si="0"/>
-        <v>1697840</v>
+        <v>75.046948592546471</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>90</v>
       </c>
@@ -35048,11 +35717,15 @@
         <v>22036.7</v>
       </c>
       <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1697840</v>
+      </c>
+      <c r="O19">
         <f t="shared" si="0"/>
-        <v>1697840</v>
+        <v>84.414310976274095</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>90</v>
       </c>
@@ -35090,11 +35763,15 @@
         <v>22036.7</v>
       </c>
       <c r="N20">
+        <f t="shared" si="1"/>
+        <v>1697840</v>
+      </c>
+      <c r="O20">
         <f t="shared" si="0"/>
-        <v>1697840</v>
+        <v>97.084933919238964</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>100</v>
       </c>
@@ -35132,11 +35809,15 @@
         <v>27436.9</v>
       </c>
       <c r="N21">
+        <f t="shared" si="1"/>
+        <v>2090450</v>
+      </c>
+      <c r="O21">
         <f t="shared" si="0"/>
-        <v>2090450</v>
+        <v>102.4748141950508</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>100</v>
       </c>
@@ -35174,11 +35855,15 @@
         <v>27436.9</v>
       </c>
       <c r="N22">
+        <f t="shared" si="1"/>
+        <v>2090450</v>
+      </c>
+      <c r="O22">
         <f t="shared" si="0"/>
-        <v>2090450</v>
+        <v>102.65257120325589</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>100</v>
       </c>
@@ -35218,6 +35903,22 @@
       <c r="N23">
         <f>B23*B23*(C23+2)+B23+50*(4*(B23+1)*(B23+1) + 2*(B23+1)+1)</f>
         <v>2090450</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>101.20892174704863</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <f>MIN(O3:O23)</f>
+        <v>72.254144693377711</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <f>MAX(O3:O23)</f>
+        <v>102.65257120325589</v>
       </c>
     </row>
   </sheetData>
@@ -35230,8 +35931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C33D06-0CE6-484F-A768-5AA8D609AD24}">
   <dimension ref="B2:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="J10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N66" sqref="N66"/>
+    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36433,10 +37134,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F18129-C50A-4531-B968-C719AE2EEC0A}">
-  <dimension ref="B2:M82"/>
+  <dimension ref="B2:M86"/>
   <sheetViews>
-    <sheetView topLeftCell="K70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q57" sqref="Q57"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="T58" sqref="T58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36448,7 +37149,7 @@
     <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
@@ -39532,6 +40233,24 @@
         <v>27436.9</v>
       </c>
     </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I85" t="s">
+        <v>22</v>
+      </c>
+      <c r="J85" s="1">
+        <f>AVERAGE(J3:J82)</f>
+        <v>380.41008749999992</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I86" t="s">
+        <v>23</v>
+      </c>
+      <c r="J86">
+        <f>SQRT(_xlfn.VAR.S(J3:J82))</f>
+        <v>13.289004409941205</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>